<commit_message>
Test pre-push hook with staging index.html
</commit_message>
<xml_diff>
--- a/data/main_data.xlsx
+++ b/data/main_data.xlsx
@@ -617,12 +617,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>f68eecd0-f353-436f-8e94-ae2383f9ab52</t>
+          <t>7a6eafab-5fa3-4f6b-9220-96f64351c8b8</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Mock 1</t>
+          <t>IBA Mock 1</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -662,7 +662,7 @@
         <v>33.33333333333333</v>
       </c>
       <c r="R2" t="n">
-        <v>31.5</v>
+        <v>22.5</v>
       </c>
       <c r="S2" t="n">
         <v>19.28571428571429</v>
@@ -695,9 +695,7 @@
       <c r="AE2" t="n">
         <v>0</v>
       </c>
-      <c r="AF2" t="n">
-        <v>9</v>
-      </c>
+      <c r="AF2" t="inlineStr"/>
       <c r="AG2" t="n">
         <v>25</v>
       </c>
@@ -719,12 +717,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>f68eecd0-f353-436f-8e94-ae2383f9ab52</t>
+          <t>7a6eafab-5fa3-4f6b-9220-96f64351c8b8</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Mock 1</t>
+          <t>IBA Mock 1</t>
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
@@ -799,12 +797,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>f68eecd0-f353-436f-8e94-ae2383f9ab52</t>
+          <t>7a6eafab-5fa3-4f6b-9220-96f64351c8b8</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Mock 1</t>
+          <t>IBA Mock 1</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -844,7 +842,7 @@
         <v>50</v>
       </c>
       <c r="R4" t="n">
-        <v>69</v>
+        <v>44.5</v>
       </c>
       <c r="S4" t="n">
         <v>28.57142857142857</v>
@@ -873,9 +871,7 @@
       <c r="AE4" t="n">
         <v>9</v>
       </c>
-      <c r="AF4" t="n">
-        <v>24.5</v>
-      </c>
+      <c r="AF4" t="inlineStr"/>
       <c r="AG4" t="n">
         <v>70</v>
       </c>
@@ -897,12 +893,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>f68eecd0-f353-436f-8e94-ae2383f9ab52</t>
+          <t>7a6eafab-5fa3-4f6b-9220-96f64351c8b8</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Mock 1</t>
+          <t>IBA Mock 1</t>
         </is>
       </c>
       <c r="F5" t="inlineStr"/>
@@ -971,12 +967,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>f68eecd0-f353-436f-8e94-ae2383f9ab52</t>
+          <t>7a6eafab-5fa3-4f6b-9220-96f64351c8b8</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Mock 1</t>
+          <t>IBA Mock 1</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -1016,13 +1012,13 @@
         <v>25</v>
       </c>
       <c r="R6" t="n">
-        <v>60.25</v>
+        <v>38.25</v>
       </c>
       <c r="S6" t="n">
         <v>23.21428571428572</v>
       </c>
       <c r="T6" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="U6" t="inlineStr"/>
       <c r="V6" t="inlineStr"/>
@@ -1045,9 +1041,7 @@
       <c r="AE6" t="n">
         <v>6.5</v>
       </c>
-      <c r="AF6" t="n">
-        <v>22</v>
-      </c>
+      <c r="AF6" t="inlineStr"/>
       <c r="AG6" t="inlineStr">
         <is>
           <t xml:space="preserve">Penalty </t>
@@ -1073,12 +1067,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>f68eecd0-f353-436f-8e94-ae2383f9ab52</t>
+          <t>7a6eafab-5fa3-4f6b-9220-96f64351c8b8</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Mock 1</t>
+          <t>IBA Mock 1</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -1118,13 +1112,13 @@
         <v>36.66666666666666</v>
       </c>
       <c r="R7" t="n">
-        <v>56.75</v>
+        <v>41.25</v>
       </c>
       <c r="S7" t="n">
         <v>36.78571428571429</v>
       </c>
       <c r="T7" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="U7" t="inlineStr"/>
       <c r="V7" t="inlineStr"/>
@@ -1147,9 +1141,7 @@
       <c r="AE7" t="n">
         <v>1.5</v>
       </c>
-      <c r="AF7" t="n">
-        <v>15.5</v>
-      </c>
+      <c r="AF7" t="inlineStr"/>
       <c r="AG7" t="inlineStr"/>
       <c r="AH7" t="inlineStr"/>
     </row>
@@ -1169,12 +1161,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>f68eecd0-f353-436f-8e94-ae2383f9ab52</t>
+          <t>7a6eafab-5fa3-4f6b-9220-96f64351c8b8</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Mock 1</t>
+          <t>IBA Mock 1</t>
         </is>
       </c>
       <c r="F8" t="inlineStr"/>
@@ -1245,12 +1237,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>f68eecd0-f353-436f-8e94-ae2383f9ab52</t>
+          <t>7a6eafab-5fa3-4f6b-9220-96f64351c8b8</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Mock 1</t>
+          <t>IBA Mock 1</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -1290,13 +1282,13 @@
         <v>26.66666666666667</v>
       </c>
       <c r="R9" t="n">
-        <v>60.25</v>
+        <v>38.75</v>
       </c>
       <c r="S9" t="n">
         <v>24.64285714285715</v>
       </c>
       <c r="T9" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="U9" t="inlineStr"/>
       <c r="V9" t="inlineStr"/>
@@ -1319,9 +1311,7 @@
       <c r="AE9" t="n">
         <v>7.5</v>
       </c>
-      <c r="AF9" t="n">
-        <v>21.5</v>
-      </c>
+      <c r="AF9" t="inlineStr"/>
       <c r="AG9" t="inlineStr"/>
       <c r="AH9" t="inlineStr"/>
     </row>
@@ -1341,12 +1331,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>f68eecd0-f353-436f-8e94-ae2383f9ab52</t>
+          <t>7a6eafab-5fa3-4f6b-9220-96f64351c8b8</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Mock 1</t>
+          <t>IBA Mock 1</t>
         </is>
       </c>
       <c r="F10" t="inlineStr"/>
@@ -1415,12 +1405,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>f68eecd0-f353-436f-8e94-ae2383f9ab52</t>
+          <t>7a6eafab-5fa3-4f6b-9220-96f64351c8b8</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Mock 1</t>
+          <t>IBA Mock 1</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -1460,13 +1450,13 @@
         <v>48.33333333333334</v>
       </c>
       <c r="R11" t="n">
-        <v>72.25</v>
+        <v>50.25</v>
       </c>
       <c r="S11" t="n">
         <v>40.35714285714286</v>
       </c>
       <c r="T11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U11" t="inlineStr"/>
       <c r="V11" t="inlineStr"/>
@@ -1489,9 +1479,7 @@
       <c r="AE11" t="n">
         <v>7</v>
       </c>
-      <c r="AF11" t="n">
-        <v>22</v>
-      </c>
+      <c r="AF11" t="inlineStr"/>
       <c r="AG11" t="inlineStr"/>
       <c r="AH11" t="inlineStr"/>
     </row>
@@ -1511,12 +1499,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>f68eecd0-f353-436f-8e94-ae2383f9ab52</t>
+          <t>7a6eafab-5fa3-4f6b-9220-96f64351c8b8</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Mock 1</t>
+          <t>IBA Mock 1</t>
         </is>
       </c>
       <c r="F12" t="inlineStr"/>
@@ -1585,12 +1573,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>f68eecd0-f353-436f-8e94-ae2383f9ab52</t>
+          <t>7a6eafab-5fa3-4f6b-9220-96f64351c8b8</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Mock 1</t>
+          <t>IBA Mock 1</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -1673,12 +1661,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>f68eecd0-f353-436f-8e94-ae2383f9ab52</t>
+          <t>7a6eafab-5fa3-4f6b-9220-96f64351c8b8</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Mock 1</t>
+          <t>IBA Mock 1</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -1753,12 +1741,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>f68eecd0-f353-436f-8e94-ae2383f9ab52</t>
+          <t>7a6eafab-5fa3-4f6b-9220-96f64351c8b8</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Mock 1</t>
+          <t>IBA Mock 1</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -1798,13 +1786,13 @@
         <v>26.66666666666667</v>
       </c>
       <c r="R15" t="n">
-        <v>72.75</v>
+        <v>47.75</v>
       </c>
       <c r="S15" t="n">
         <v>32.5</v>
       </c>
       <c r="T15" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U15" t="inlineStr"/>
       <c r="V15" t="inlineStr"/>
@@ -1827,9 +1815,7 @@
       <c r="AE15" t="n">
         <v>8.5</v>
       </c>
-      <c r="AF15" t="n">
-        <v>25</v>
-      </c>
+      <c r="AF15" t="inlineStr"/>
       <c r="AG15" t="inlineStr"/>
       <c r="AH15" t="inlineStr"/>
     </row>
@@ -1849,12 +1835,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>f68eecd0-f353-436f-8e94-ae2383f9ab52</t>
+          <t>7a6eafab-5fa3-4f6b-9220-96f64351c8b8</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Mock 1</t>
+          <t>IBA Mock 1</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -1894,13 +1880,13 @@
         <v>26.66666666666667</v>
       </c>
       <c r="R16" t="n">
-        <v>69.25</v>
+        <v>48.25</v>
       </c>
       <c r="S16" t="n">
         <v>38.92857142857143</v>
       </c>
       <c r="T16" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="U16" t="inlineStr"/>
       <c r="V16" t="inlineStr"/>
@@ -1923,9 +1909,7 @@
       <c r="AE16" t="n">
         <v>7</v>
       </c>
-      <c r="AF16" t="n">
-        <v>21</v>
-      </c>
+      <c r="AF16" t="inlineStr"/>
       <c r="AG16" t="inlineStr"/>
       <c r="AH16" t="inlineStr"/>
     </row>
@@ -1945,12 +1929,12 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>f68eecd0-f353-436f-8e94-ae2383f9ab52</t>
+          <t>7a6eafab-5fa3-4f6b-9220-96f64351c8b8</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Mock 1</t>
+          <t>IBA Mock 1</t>
         </is>
       </c>
       <c r="F17" t="inlineStr"/>
@@ -2019,12 +2003,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>f68eecd0-f353-436f-8e94-ae2383f9ab52</t>
+          <t>7a6eafab-5fa3-4f6b-9220-96f64351c8b8</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Mock 1</t>
+          <t>IBA Mock 1</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -2064,7 +2048,7 @@
         <v>-1.666666666666667</v>
       </c>
       <c r="R18" t="n">
-        <v>43.25</v>
+        <v>29.25</v>
       </c>
       <c r="S18" t="n">
         <v>21.78571428571428</v>
@@ -2093,9 +2077,7 @@
       <c r="AE18" t="n">
         <v>1.5</v>
       </c>
-      <c r="AF18" t="n">
-        <v>14</v>
-      </c>
+      <c r="AF18" t="inlineStr"/>
       <c r="AG18" t="inlineStr"/>
       <c r="AH18" t="inlineStr"/>
     </row>
@@ -2115,12 +2097,12 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>f68eecd0-f353-436f-8e94-ae2383f9ab52</t>
+          <t>7a6eafab-5fa3-4f6b-9220-96f64351c8b8</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Mock 1</t>
+          <t>IBA Mock 1</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -2160,7 +2142,7 @@
         <v>40</v>
       </c>
       <c r="R19" t="n">
-        <v>69.5</v>
+        <v>48</v>
       </c>
       <c r="S19" t="n">
         <v>37.85714285714285</v>
@@ -2189,9 +2171,7 @@
       <c r="AE19" t="n">
         <v>7.5</v>
       </c>
-      <c r="AF19" t="n">
-        <v>21.5</v>
-      </c>
+      <c r="AF19" t="inlineStr"/>
       <c r="AG19" t="inlineStr"/>
       <c r="AH19" t="inlineStr"/>
     </row>
@@ -2211,12 +2191,12 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>f68eecd0-f353-436f-8e94-ae2383f9ab52</t>
+          <t>7a6eafab-5fa3-4f6b-9220-96f64351c8b8</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Mock 1</t>
+          <t>IBA Mock 1</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -2256,7 +2236,7 @@
         <v>41.66666666666667</v>
       </c>
       <c r="R20" t="n">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="S20" t="n">
         <v>28.57142857142857</v>
@@ -2285,9 +2265,7 @@
       <c r="AE20" t="n">
         <v>0</v>
       </c>
-      <c r="AF20" t="n">
-        <v>14</v>
-      </c>
+      <c r="AF20" t="inlineStr"/>
       <c r="AG20" t="inlineStr"/>
       <c r="AH20" t="inlineStr"/>
     </row>
@@ -2307,12 +2285,12 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>f68eecd0-f353-436f-8e94-ae2383f9ab52</t>
+          <t>7a6eafab-5fa3-4f6b-9220-96f64351c8b8</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Mock 1</t>
+          <t>IBA Mock 1</t>
         </is>
       </c>
       <c r="F21" t="inlineStr"/>
@@ -2363,12 +2341,12 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>f68eecd0-f353-436f-8e94-ae2383f9ab52</t>
+          <t>7a6eafab-5fa3-4f6b-9220-96f64351c8b8</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Mock 1</t>
+          <t>IBA Mock 1</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -2408,13 +2386,13 @@
         <v>56.66666666666666</v>
       </c>
       <c r="R22" t="n">
-        <v>55.75</v>
+        <v>42.25</v>
       </c>
       <c r="S22" t="n">
         <v>41.07142857142857</v>
       </c>
       <c r="T22" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="U22" t="inlineStr"/>
       <c r="V22" t="inlineStr"/>
@@ -2437,9 +2415,7 @@
       <c r="AE22" t="n">
         <v>7</v>
       </c>
-      <c r="AF22" t="n">
-        <v>13.5</v>
-      </c>
+      <c r="AF22" t="inlineStr"/>
       <c r="AG22" t="inlineStr"/>
       <c r="AH22" t="inlineStr"/>
     </row>

</xml_diff>